<commit_message>
Add Check Indent option in preference
</commit_message>
<xml_diff>
--- a/Rules.xlsx
+++ b/Rules.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$15</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -555,10 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -594,7 +598,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -607,7 +611,7 @@
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -624,7 +628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -634,10 +638,14 @@
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -650,7 +658,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -663,7 +671,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -676,7 +684,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -702,7 +710,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -717,7 +725,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -732,7 +740,7 @@
       </c>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -745,18 +753,18 @@
       </c>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -767,38 +775,38 @@
       <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E15">
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A3:D16">
     <sortCondition ref="A3"/>
   </sortState>

</xml_diff>